<commit_message>
Update Estadisticas CUT. 1953-2021.xlsx
</commit_message>
<xml_diff>
--- a/Estadisticas CUT. 1953-2021.xlsx
+++ b/Estadisticas CUT. 1953-2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebao\Dropbox\2021\CIPSTRA\Dataset\Minuta 3. Series de afiliación CUT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebao\Documents\GitHub\Series-CUT-1953-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1048374-7239-48D6-80B1-30B1D34E37A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84ADC21-1DC7-4D0C-A9B1-1F4382D58847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leeme" sheetId="5" r:id="rId1"/>
@@ -249,32 +249,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Fuente: Elaboración propia en base a Marchant, Felipe (2021): "Afiliación sindical y tamaño de sindicatos, 1990-2020". En </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Repositorio de Estadísticas Sindicales, 1900-2020</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">AUTOR (2021): "Nombre de la tabla". En </t>
     </r>
     <r>
@@ -375,32 +349,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Se refiere a la utilización de más de una tabla o base de datos en un trabajo, y para citar al final de un trabajo como parte de las referencias bibliográficas.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Osorio, Sebastián (2021): "Afiliación anual de la Central Unitaria de Trabajadores, 1988-2020". En </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Repositorio de Estadísticas Sindicales, 1900-2020</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. CIPSTRA, GETSUR y VVAA. Disponible en: https://repositoriosindical.netlify.app/</t>
     </r>
   </si>
   <si>
@@ -715,8 +663,44 @@
     <t>Resultados de elecciones CUT por Listas, 1988-2021</t>
   </si>
   <si>
+    <t>Partido Radical (PR)</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>11.61%</t>
+  </si>
+  <si>
+    <t>Acta sobre representación a XII Congreso Nacional CUT 2020</t>
+  </si>
+  <si>
+    <t>Resultados de elecciones CUT y CUT Chile para principales partidos políticos, 1953-2021</t>
+  </si>
+  <si>
+    <t>Fuentes:</t>
+  </si>
+  <si>
+    <t>Angell, A. (1974): Partidos políticos y movimiento obrero en Chile. De los orígenes hasta el triunfo de la Unidad Popular, Ciudad de México: Ediciones ERA. Pp. 221-224</t>
+  </si>
+  <si>
+    <t>Farías, Victor (2000): La izquierda chilena (1969-1973): Documentos para el estudio de su línea estratégica. Santiago de Chile, Centro de Estudios Públicos. P. 2867-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osorio, Sebastián (2015): Trayectoria y cambios en la política del movimiento sindical en Chile, 1990-2010. El caso de la CUT, entre la independencia política y la integración al bloque histórico neoliberal. Tesis para optar al grado de Magíster en Historia de Chile, Universidad de Santiago. </t>
+  </si>
+  <si>
+    <t>Repositorio de Estadísticas Sindicales</t>
+  </si>
+  <si>
+    <t>Última actualización: 19/05/2021</t>
+  </si>
+  <si>
+    <t>Osorio, Sebastián (2021): "Resultados de elecciones CUT por listas, 1988-2021". En Repositorio de Estadísticas Sindicales, 1900-2020. CIPSTRA, GETSUR y VVAA. Disponible en: https://repositoriosindical.netlify.app/</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Osorio, Sebastián (2021): "Resultados de elecciones CUT por listas, 1988-2021". En </t>
+      <t xml:space="preserve">Fuente: Elaboración propia en base a Osorio, Sebastián (2021): "Afiliación sindical y tamaño de sindicatos, 1990-2020". En </t>
     </r>
     <r>
       <rPr>
@@ -737,24 +721,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>. CIPSTRA, GETSUR y VVAA. Disponible en: https://repositoriosindical.netlify.app/</t>
+      <t xml:space="preserve">. </t>
     </r>
   </si>
   <si>
-    <t>Partido Radical (PR)</t>
-  </si>
-  <si>
-    <t>Otros</t>
-  </si>
-  <si>
-    <t>11.61%</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Osorio, Sebastián (2021): "Resultados de elecciones CUT para principales partidos políticos, 1988-2021". En </t>
+      <t xml:space="preserve">Osorio, Sebastián (2021): "Afiliación anual de la Central Unitaria de Trabajadores, 1988-2020". En </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <i/>
         <sz val="11"/>
         <color theme="1"/>
@@ -766,6 +742,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -776,31 +753,60 @@
     </r>
   </si>
   <si>
-    <t>Acta sobre representación a XII Congreso Nacional CUT 2020</t>
-  </si>
-  <si>
-    <t>Resultados de elecciones CUT y CUT Chile para principales partidos políticos, 1953-2021</t>
-  </si>
-  <si>
-    <t>Fuentes:</t>
-  </si>
-  <si>
-    <t>Angell, A. (1974): Partidos políticos y movimiento obrero en Chile. De los orígenes hasta el triunfo de la Unidad Popular, Ciudad de México: Ediciones ERA. Pp. 221-224</t>
-  </si>
-  <si>
-    <t>Farías, Victor (2000): La izquierda chilena (1969-1973): Documentos para el estudio de su línea estratégica. Santiago de Chile, Centro de Estudios Públicos. P. 2867-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osorio, Sebastián (2015): Trayectoria y cambios en la política del movimiento sindical en Chile, 1990-2010. El caso de la CUT, entre la independencia política y la integración al bloque histórico neoliberal. Tesis para optar al grado de Magíster en Historia de Chile, Universidad de Santiago. </t>
-  </si>
-  <si>
-    <t>Repositorio de Estadísticas Sindicales</t>
-  </si>
-  <si>
-    <t>Última actualización: 19/05/2021</t>
-  </si>
-  <si>
-    <t>Osorio, Sebastián (2021): "Resultados de elecciones CUT por listas, 1988-2021". En Repositorio de Estadísticas Sindicales, 1900-2020. CIPSTRA, GETSUR y VVAA. Disponible en: https://repositoriosindical.netlify.app/</t>
+    <r>
+      <t xml:space="preserve">Osorio, Sebastián (2021): "Resultados de elecciones CUT por listas, 1988-2021". En </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repositorio de Estadísticas Sindicales, 1900-2020</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. CIPSTRA, GETSUR y VVAA. Disponible en: https://repositoriosindical.netlify.app/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Osorio, Sebastián (2021): "Resultados de elecciones CUT para principales partidos políticos, 1953-2021". En </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repositorio de Estadísticas Sindicales, 1900-2020</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. CIPSTRA, GETSUR y VVAA. Disponible en: https://repositoriosindical.netlify.app/</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -810,7 +816,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -863,6 +869,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -872,7 +887,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1168,37 +1183,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1241,7 +1225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1454,66 +1438,27 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1522,14 +1467,47 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1814,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB901A23-7AF2-449C-A861-55C245B6AB57}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1825,7 +1803,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1861,7 +1839,7 @@
     </row>
     <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
@@ -1874,7 +1852,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
@@ -1884,7 +1862,7 @@
     </row>
     <row r="14" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
@@ -1892,12 +1870,12 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -1905,7 +1883,7 @@
     </row>
     <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1924,7 +1902,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1935,14 +1913,14 @@
     <col min="4" max="4" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
+      <c r="B1" s="89"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1956,7 +1934,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -2064,10 +2042,10 @@
         <v>1998</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2224,7 +2202,7 @@
         <v>716696</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E26" s="1"/>
     </row>
@@ -2292,7 +2270,7 @@
         <v>740000</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -2310,7 +2288,7 @@
         <v>740000</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2329,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9167BEA-94A8-4989-8B01-EDCD53765F3A}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2342,77 +2320,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="83" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="27" t="s">
-        <v>136</v>
+      <c r="A1" s="91" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="100" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="102"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="102"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="102"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="102"/>
-      <c r="B5" s="102"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="83">
+      <c r="A6" s="91">
         <v>1988</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="85"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="93"/>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="20">
         <v>57198</v>
@@ -2427,12 +2405,12 @@
         <v>3</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="52" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="20">
         <v>106192</v>
@@ -2449,7 +2427,7 @@
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="20">
         <v>74180</v>
@@ -2466,7 +2444,7 @@
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="52" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="20">
         <v>52288</v>
@@ -2483,7 +2461,7 @@
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" s="36">
         <v>289858</v>
@@ -2500,37 +2478,37 @@
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="86">
+      <c r="A14" s="94">
         <v>1991</v>
       </c>
-      <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="88"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="96"/>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="61" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="58" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" s="41">
         <v>16368</v>
@@ -2545,12 +2523,12 @@
         <v>0</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="59" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" s="41">
         <v>227568</v>
@@ -2559,7 +2537,7 @@
         <v>0.43099999999999999</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="42">
         <v>5</v>
@@ -2567,7 +2545,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="41">
         <v>104016</v>
@@ -2584,7 +2562,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="41">
         <v>184272</v>
@@ -2601,7 +2579,7 @@
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="43">
         <v>528000</v>
@@ -2618,37 +2596,37 @@
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="86">
+      <c r="A22" s="94">
         <v>1996</v>
       </c>
-      <c r="B22" s="87"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="88"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
     </row>
     <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="64" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B24" s="41">
         <v>153734</v>
@@ -2663,12 +2641,12 @@
         <v>5</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="41">
         <v>155393</v>
@@ -2685,7 +2663,7 @@
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" s="41">
         <v>34839</v>
@@ -2702,7 +2680,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="64" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" s="41">
         <v>193550</v>
@@ -2719,7 +2697,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="64" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="41">
         <v>15484</v>
@@ -2736,7 +2714,7 @@
     </row>
     <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="43">
         <v>553000</v>
@@ -2753,37 +2731,37 @@
     </row>
     <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="86">
+      <c r="A31" s="94">
         <v>1998</v>
       </c>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="88"/>
+      <c r="B31" s="95"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="96"/>
     </row>
     <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D32" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E32" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="64" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B33" s="41">
         <v>12266</v>
@@ -2798,12 +2776,12 @@
         <v>1</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="64" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" s="41">
         <v>29758</v>
@@ -2820,13 +2798,13 @@
     </row>
     <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D35" s="40">
         <v>0</v>
@@ -2837,13 +2815,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="64" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D36" s="40">
         <v>0</v>
@@ -2854,13 +2832,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="64" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D37" s="40">
         <v>0</v>
@@ -2872,7 +2850,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="64" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B38" s="41">
         <v>45871</v>
@@ -2889,7 +2867,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="64" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B39" s="41">
         <v>60753</v>
@@ -2906,7 +2884,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="64" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40" s="41">
         <v>15050</v>
@@ -2923,13 +2901,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="64" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C41" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D41" s="40">
         <v>0</v>
@@ -2940,7 +2918,7 @@
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B42" s="43">
         <v>171176</v>
@@ -2957,37 +2935,37 @@
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="86">
+      <c r="A44" s="94">
         <v>2000</v>
       </c>
-      <c r="B44" s="87"/>
-      <c r="C44" s="87"/>
-      <c r="D44" s="87"/>
-      <c r="E44" s="88"/>
+      <c r="B44" s="95"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="96"/>
     </row>
     <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D45" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E45" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B46" s="32">
         <v>76644</v>
@@ -3002,12 +2980,12 @@
         <v>4</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B47" s="32">
         <v>140087</v>
@@ -3016,7 +2994,7 @@
         <v>0.47589999999999999</v>
       </c>
       <c r="D47" s="50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E47" s="35">
         <v>7</v>
@@ -3024,7 +3002,7 @@
     </row>
     <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="64" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B48" s="32">
         <v>4875</v>
@@ -3042,7 +3020,7 @@
     </row>
     <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B49" s="32">
         <v>72774</v>
@@ -3059,7 +3037,7 @@
     </row>
     <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B50" s="43">
         <v>294380</v>
@@ -3076,37 +3054,37 @@
     </row>
     <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="86">
+      <c r="A52" s="94">
         <v>2004</v>
       </c>
-      <c r="B52" s="87"/>
-      <c r="C52" s="87"/>
-      <c r="D52" s="87"/>
-      <c r="E52" s="88"/>
+      <c r="B52" s="95"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="96"/>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C53" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D53" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E53" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="64" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B54" s="32">
         <v>229891</v>
@@ -3121,12 +3099,12 @@
         <v>5</v>
       </c>
       <c r="F54" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="64" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B55" s="32">
         <v>60754</v>
@@ -3143,7 +3121,7 @@
     </row>
     <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B56" s="32">
         <v>102657</v>
@@ -3160,7 +3138,7 @@
     </row>
     <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="64" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B57" s="32">
         <v>252575</v>
@@ -3177,7 +3155,7 @@
     </row>
     <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B58" s="32">
         <v>32183</v>
@@ -3194,7 +3172,7 @@
     </row>
     <row r="59" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B59" s="43">
         <v>678060</v>
@@ -3212,37 +3190,37 @@
     </row>
     <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="86">
+      <c r="A61" s="94">
         <v>2008</v>
       </c>
-      <c r="B61" s="87"/>
-      <c r="C61" s="87"/>
-      <c r="D61" s="87"/>
-      <c r="E61" s="88"/>
+      <c r="B61" s="95"/>
+      <c r="C61" s="95"/>
+      <c r="D61" s="95"/>
+      <c r="E61" s="96"/>
     </row>
     <row r="62" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B62" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C62" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D62" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E62" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="64" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B63" s="32">
         <v>17073</v>
@@ -3257,12 +3235,12 @@
         <v>0</v>
       </c>
       <c r="F63" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B64" s="32">
         <v>6325</v>
@@ -3279,7 +3257,7 @@
     </row>
     <row r="65" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="64" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B65" s="32">
         <v>73541</v>
@@ -3296,7 +3274,7 @@
     </row>
     <row r="66" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B66" s="32">
         <v>324674</v>
@@ -3313,7 +3291,7 @@
     </row>
     <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B67" s="32">
         <v>247078</v>
@@ -3330,7 +3308,7 @@
     </row>
     <row r="68" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="64" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B68" s="32">
         <v>39130</v>
@@ -3348,7 +3326,7 @@
     </row>
     <row r="69" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B69" s="32">
         <v>4493</v>
@@ -3365,7 +3343,7 @@
     </row>
     <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B70" s="43">
         <v>712314</v>
@@ -3382,37 +3360,37 @@
     </row>
     <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="86">
+      <c r="A72" s="94">
         <v>2012</v>
       </c>
-      <c r="B72" s="87"/>
-      <c r="C72" s="87"/>
-      <c r="D72" s="87"/>
-      <c r="E72" s="88"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="95"/>
+      <c r="D72" s="95"/>
+      <c r="E72" s="96"/>
     </row>
     <row r="73" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B73" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C73" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D73" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E73" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F73" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="64" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B74" s="32">
         <v>98043</v>
@@ -3429,7 +3407,7 @@
     </row>
     <row r="75" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="64" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B75" s="32">
         <v>321028</v>
@@ -3446,7 +3424,7 @@
     </row>
     <row r="76" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="64" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B76" s="32">
         <v>6431</v>
@@ -3463,7 +3441,7 @@
     </row>
     <row r="77" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="64" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B77" s="32">
         <v>291194</v>
@@ -3481,7 +3459,7 @@
     </row>
     <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B78" s="48">
         <v>716696</v>
@@ -3498,37 +3476,37 @@
     </row>
     <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="86">
+      <c r="A80" s="94">
         <v>2016</v>
       </c>
-      <c r="B80" s="87"/>
-      <c r="C80" s="87"/>
-      <c r="D80" s="87"/>
-      <c r="E80" s="88"/>
+      <c r="B80" s="95"/>
+      <c r="C80" s="95"/>
+      <c r="D80" s="95"/>
+      <c r="E80" s="96"/>
     </row>
     <row r="81" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B81" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C81" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D81" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E81" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F81" s="27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82" s="64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B82" s="33">
         <v>22500</v>
@@ -3540,12 +3518,12 @@
         <v>1</v>
       </c>
       <c r="E82" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B83" s="33">
         <v>22500</v>
@@ -3557,12 +3535,12 @@
         <v>1</v>
       </c>
       <c r="E83" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="64" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B84" s="33">
         <v>66000</v>
@@ -3574,46 +3552,46 @@
         <v>8</v>
       </c>
       <c r="E84" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="64" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C85" s="49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D85" s="40">
         <v>0</v>
       </c>
       <c r="E85" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B86" s="33">
         <v>253000</v>
       </c>
       <c r="C86" s="49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D86" s="40">
         <v>16</v>
       </c>
       <c r="E86" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B87" s="33">
         <v>286000</v>
@@ -3625,12 +3603,12 @@
         <v>19</v>
       </c>
       <c r="E87" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B88" s="43">
         <v>660000</v>
@@ -3642,42 +3620,42 @@
         <v>45</v>
       </c>
       <c r="E88" s="39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="90" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="86">
+      <c r="A90" s="94">
         <v>2017</v>
       </c>
-      <c r="B90" s="87"/>
-      <c r="C90" s="87"/>
-      <c r="D90" s="87"/>
-      <c r="E90" s="88"/>
+      <c r="B90" s="95"/>
+      <c r="C90" s="95"/>
+      <c r="D90" s="95"/>
+      <c r="E90" s="96"/>
     </row>
     <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B91" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C91" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D91" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E91" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F91" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B92" s="33">
         <v>2123</v>
@@ -3694,7 +3672,7 @@
     </row>
     <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B93" s="33">
         <v>59891</v>
@@ -3711,7 +3689,7 @@
     </row>
     <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B94" s="33">
         <v>387667</v>
@@ -3728,7 +3706,7 @@
     </row>
     <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B95" s="33">
         <v>31345</v>
@@ -3745,7 +3723,7 @@
     </row>
     <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B96" s="33">
         <v>293382</v>
@@ -3762,7 +3740,7 @@
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B97" s="36">
         <v>774408</v>
@@ -3799,8 +3777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE4BC51-3CF1-4DE8-AB3C-8C25665AE275}">
   <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3810,17 +3788,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="89" t="s">
-        <v>142</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="91"/>
-      <c r="J1" s="27" t="s">
-        <v>140</v>
+      <c r="B1" s="91" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="100" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3831,7 +3810,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="77" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E2" s="77" t="s">
         <v>6</v>
@@ -3840,185 +3819,185 @@
         <v>7</v>
       </c>
       <c r="G2" s="77" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H2" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="94" t="s">
-        <v>143</v>
+        <v>52</v>
+      </c>
+      <c r="I2" s="82" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="78">
         <v>1953</v>
       </c>
-      <c r="C3" s="95">
+      <c r="C3" s="83">
         <v>6.3E-2</v>
       </c>
-      <c r="D3" s="95">
+      <c r="D3" s="83">
         <v>6.3E-2</v>
       </c>
-      <c r="E3" s="95">
+      <c r="E3" s="83">
         <v>0.21299999999999999</v>
       </c>
-      <c r="F3" s="95">
+      <c r="F3" s="83">
         <v>0.253</v>
       </c>
-      <c r="G3" s="95">
+      <c r="G3" s="83">
         <v>0.40800000000000003</v>
       </c>
-      <c r="H3" s="92">
+      <c r="H3" s="80">
         <v>1</v>
       </c>
-      <c r="I3" s="96" t="s">
-        <v>144</v>
+      <c r="I3" s="97" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="78">
         <v>1957</v>
       </c>
-      <c r="C4" s="95">
+      <c r="C4" s="83">
         <v>0.14699999999999999</v>
       </c>
-      <c r="D4" s="95">
+      <c r="D4" s="83">
         <v>0.09</v>
       </c>
-      <c r="E4" s="95">
+      <c r="E4" s="83">
         <v>0.39900000000000002</v>
       </c>
-      <c r="F4" s="95">
+      <c r="F4" s="83">
         <v>0.25900000000000001</v>
       </c>
-      <c r="G4" s="95">
+      <c r="G4" s="83">
         <v>0.10500000000000001</v>
       </c>
-      <c r="H4" s="92">
+      <c r="H4" s="80">
         <v>1</v>
       </c>
-      <c r="I4" s="96"/>
+      <c r="I4" s="97"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="78">
         <v>1959</v>
       </c>
-      <c r="C5" s="95">
+      <c r="C5" s="83">
         <v>0.14599999999999999</v>
       </c>
-      <c r="D5" s="95">
+      <c r="D5" s="83">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="E5" s="95">
+      <c r="E5" s="83">
         <v>0.44700000000000001</v>
       </c>
-      <c r="F5" s="95">
+      <c r="F5" s="83">
         <v>0.28100000000000003</v>
       </c>
-      <c r="G5" s="95">
+      <c r="G5" s="83">
         <v>8.4999999999999964E-2</v>
       </c>
-      <c r="H5" s="92">
+      <c r="H5" s="80">
         <v>1</v>
       </c>
-      <c r="I5" s="96"/>
+      <c r="I5" s="97"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="78">
         <v>1962</v>
       </c>
-      <c r="C6" s="95">
+      <c r="C6" s="83">
         <v>0.17899999999999999</v>
       </c>
-      <c r="D6" s="95">
+      <c r="D6" s="83">
         <v>6.2E-2</v>
       </c>
-      <c r="E6" s="95">
+      <c r="E6" s="83">
         <v>0.311</v>
       </c>
-      <c r="F6" s="95">
+      <c r="F6" s="83">
         <v>0.28399999999999997</v>
       </c>
-      <c r="G6" s="95">
+      <c r="G6" s="83">
         <v>0.16399999999999998</v>
       </c>
-      <c r="H6" s="92">
+      <c r="H6" s="80">
         <v>1</v>
       </c>
-      <c r="I6" s="96"/>
+      <c r="I6" s="97"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="78">
         <v>1965</v>
       </c>
-      <c r="C7" s="95">
+      <c r="C7" s="83">
         <v>0.11899999999999999</v>
       </c>
-      <c r="D7" s="95">
+      <c r="D7" s="83">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E7" s="95">
+      <c r="E7" s="83">
         <v>0.42299999999999999</v>
       </c>
-      <c r="F7" s="95">
+      <c r="F7" s="83">
         <v>0.33100000000000002</v>
       </c>
-      <c r="G7" s="95">
+      <c r="G7" s="83">
         <v>7.900000000000007E-2</v>
       </c>
-      <c r="H7" s="92">
+      <c r="H7" s="80">
         <v>1</v>
       </c>
-      <c r="I7" s="96"/>
+      <c r="I7" s="97"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="78">
         <v>1968</v>
       </c>
-      <c r="C8" s="95">
+      <c r="C8" s="83">
         <v>0.10199999999999999</v>
       </c>
-      <c r="D8" s="95">
+      <c r="D8" s="83">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="E8" s="95">
+      <c r="E8" s="83">
         <v>0.45500000000000002</v>
       </c>
-      <c r="F8" s="95">
+      <c r="F8" s="83">
         <v>0.246</v>
       </c>
-      <c r="G8" s="95">
+      <c r="G8" s="83">
         <v>0.11600000000000001</v>
       </c>
-      <c r="H8" s="92">
+      <c r="H8" s="80">
         <v>1</v>
       </c>
-      <c r="I8" s="96"/>
+      <c r="I8" s="97"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="78">
         <v>1972</v>
       </c>
-      <c r="C9" s="95">
+      <c r="C9" s="83">
         <v>0.27100000000000002</v>
       </c>
-      <c r="D9" s="95">
+      <c r="D9" s="83">
         <v>4.0099999999999997E-2</v>
       </c>
-      <c r="E9" s="95">
+      <c r="E9" s="83">
         <v>0.31680000000000003</v>
       </c>
-      <c r="F9" s="95">
+      <c r="F9" s="83">
         <v>0.2712</v>
       </c>
-      <c r="G9" s="95">
+      <c r="G9" s="83">
         <v>0.10089999999999999</v>
       </c>
-      <c r="H9" s="92">
+      <c r="H9" s="80">
         <v>1</v>
       </c>
-      <c r="I9" s="97" t="s">
-        <v>145</v>
+      <c r="I9" s="84" t="s">
+        <v>141</v>
       </c>
       <c r="J9" s="3"/>
     </row>
@@ -4026,223 +4005,223 @@
       <c r="B10" s="72">
         <v>1988</v>
       </c>
-      <c r="C10" s="98">
+      <c r="C10" s="85">
         <v>0.36599999999999999</v>
       </c>
-      <c r="D10" s="98">
+      <c r="D10" s="85">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="E10" s="98">
+      <c r="E10" s="85">
         <v>0.222</v>
       </c>
-      <c r="F10" s="98">
+      <c r="F10" s="85">
         <v>0.24099999999999999</v>
       </c>
-      <c r="G10" s="98">
+      <c r="G10" s="85">
         <v>0.13400000000000001</v>
       </c>
-      <c r="H10" s="92">
+      <c r="H10" s="80">
         <v>1</v>
       </c>
-      <c r="I10" s="96" t="s">
-        <v>146</v>
+      <c r="I10" s="97" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="72">
         <v>1991</v>
       </c>
-      <c r="C11" s="98">
+      <c r="C11" s="85">
         <v>0.32300000000000001</v>
       </c>
-      <c r="D11" s="98">
+      <c r="D11" s="85">
         <v>4.3099999999999999E-2</v>
       </c>
-      <c r="E11" s="98">
+      <c r="E11" s="85">
         <v>0.19700000000000001</v>
       </c>
-      <c r="F11" s="98">
+      <c r="F11" s="85">
         <v>0.34899999999999998</v>
       </c>
-      <c r="G11" s="98">
+      <c r="G11" s="85">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="H11" s="92">
+      <c r="H11" s="80">
         <v>1</v>
       </c>
-      <c r="I11" s="96"/>
+      <c r="I11" s="97"/>
       <c r="J11" s="70"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="72">
         <v>1996</v>
       </c>
-      <c r="C12" s="98">
+      <c r="C12" s="85">
         <v>0.25800000000000001</v>
       </c>
-      <c r="D12" s="98">
+      <c r="D12" s="85">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E12" s="98">
+      <c r="E12" s="85">
         <v>0.28100000000000003</v>
       </c>
-      <c r="F12" s="98">
+      <c r="F12" s="85">
         <v>0.34100000000000003</v>
       </c>
-      <c r="G12" s="98">
+      <c r="G12" s="85">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="H12" s="92">
+      <c r="H12" s="80">
         <v>1</v>
       </c>
-      <c r="I12" s="96"/>
+      <c r="I12" s="97"/>
       <c r="J12" s="71"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="72">
         <v>1998</v>
       </c>
-      <c r="C13" s="98">
+      <c r="C13" s="85">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="D13" s="98">
+      <c r="D13" s="85">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="E13" s="98">
+      <c r="E13" s="85">
         <v>0.35499999999999998</v>
       </c>
-      <c r="F13" s="98">
+      <c r="F13" s="85">
         <v>0.442</v>
       </c>
-      <c r="G13" s="98">
+      <c r="G13" s="85">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="H13" s="92">
+      <c r="H13" s="80">
         <v>1</v>
       </c>
-      <c r="I13" s="96"/>
+      <c r="I13" s="97"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="72">
         <v>2000</v>
       </c>
-      <c r="C14" s="98">
+      <c r="C14" s="85">
         <v>0.216</v>
       </c>
-      <c r="D14" s="98">
+      <c r="D14" s="85">
         <v>6.4799999999999996E-2</v>
       </c>
-      <c r="E14" s="98">
+      <c r="E14" s="85">
         <v>0.2472</v>
       </c>
-      <c r="F14" s="98">
+      <c r="F14" s="85">
         <v>0.45500000000000002</v>
       </c>
-      <c r="G14" s="98">
+      <c r="G14" s="85">
         <v>1.66E-2</v>
       </c>
-      <c r="H14" s="92">
+      <c r="H14" s="80">
         <v>1</v>
       </c>
-      <c r="I14" s="96"/>
+      <c r="I14" s="97"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="72">
         <v>2004</v>
       </c>
-      <c r="C15" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="98">
+      <c r="C15" s="85" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="85">
         <v>3.49E-2</v>
       </c>
-      <c r="E15" s="98">
+      <c r="E15" s="85">
         <v>0.33900000000000002</v>
       </c>
-      <c r="F15" s="98">
+      <c r="F15" s="85">
         <v>0.42</v>
       </c>
-      <c r="G15" s="98">
+      <c r="G15" s="85">
         <v>0.24099999999999999</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="80">
         <v>1</v>
       </c>
-      <c r="I15" s="96"/>
+      <c r="I15" s="97"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="72">
         <v>2008</v>
       </c>
-      <c r="C16" s="98">
+      <c r="C16" s="85">
         <v>0.11210000000000001</v>
       </c>
-      <c r="D16" s="99">
+      <c r="D16" s="86">
         <v>0</v>
       </c>
-      <c r="E16" s="98">
+      <c r="E16" s="85">
         <v>0.35420000000000001</v>
       </c>
-      <c r="F16" s="98">
+      <c r="F16" s="85">
         <v>0.44700000000000001</v>
       </c>
-      <c r="G16" s="98">
+      <c r="G16" s="85">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="H16" s="92">
+      <c r="H16" s="80">
         <v>1</v>
       </c>
-      <c r="I16" s="96"/>
+      <c r="I16" s="97"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="72">
         <v>2012</v>
       </c>
-      <c r="C17" s="98">
+      <c r="C17" s="85">
         <v>0.13700000000000001</v>
       </c>
-      <c r="D17" s="99">
+      <c r="D17" s="86">
         <v>0</v>
       </c>
-      <c r="E17" s="98">
+      <c r="E17" s="85">
         <v>0.44800000000000001</v>
       </c>
-      <c r="F17" s="98">
+      <c r="F17" s="85">
         <v>0.40600000000000003</v>
       </c>
-      <c r="G17" s="98">
+      <c r="G17" s="85">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H17" s="92">
+      <c r="H17" s="80">
         <v>1</v>
       </c>
-      <c r="I17" s="100" t="s">
-        <v>149</v>
+      <c r="I17" s="98" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="72">
         <v>2016</v>
       </c>
-      <c r="C18" s="99">
+      <c r="C18" s="86">
         <v>0.1</v>
       </c>
-      <c r="D18" s="99">
+      <c r="D18" s="86">
         <v>0</v>
       </c>
-      <c r="E18" s="98">
+      <c r="E18" s="85">
         <v>0.38300000000000001</v>
       </c>
-      <c r="F18" s="98">
+      <c r="F18" s="85">
         <v>0.433</v>
       </c>
-      <c r="G18" s="99">
+      <c r="G18" s="86">
         <v>0.08</v>
       </c>
-      <c r="H18" s="92">
+      <c r="H18" s="80">
         <v>1</v>
       </c>
-      <c r="I18" s="100"/>
+      <c r="I18" s="98"/>
     </row>
     <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="73">
@@ -4263,10 +4242,10 @@
       <c r="G19" s="75">
         <v>0.1215</v>
       </c>
-      <c r="H19" s="93">
+      <c r="H19" s="81">
         <v>1</v>
       </c>
-      <c r="I19" s="101"/>
+      <c r="I19" s="99"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C20" s="69"/>
@@ -4324,10 +4303,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:H1"/>
     <mergeCell ref="I3:I8"/>
     <mergeCell ref="I10:I16"/>
     <mergeCell ref="I17:I19"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>